<commit_message>
Add other contacts matrices
</commit_message>
<xml_diff>
--- a/topics/covid19/current-patterns-transmission/reports/20200327_comix_social_contacts.xlsx
+++ b/topics/covid19/current-patterns-transmission/reports/20200327_comix_social_contacts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsh301231\Documents\projects\covid_projects\contact_survey_2020\outputs\contact_matrices_online\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsh301231\Documents\projects\covid_projects\cmmid.github.io\topics\covid19\current-patterns-transmission\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6183AE-0465-4030-B3E1-6AD20BAD4A44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1855A2E-AD49-4DC0-B112-ADAB6742E44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{D97C3AA1-9ED6-42D7-923F-BF8E97FEF53A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D97C3AA1-9ED6-42D7-923F-BF8E97FEF53A}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,12 @@
     <sheet name="Physical_contacts" sheetId="3" r:id="rId3"/>
     <sheet name="All_contacts_imputed" sheetId="4" r:id="rId4"/>
     <sheet name="Physical_contacts_imputed" sheetId="5" r:id="rId5"/>
+    <sheet name="All_contacts_home" sheetId="6" r:id="rId6"/>
+    <sheet name="All_contacts_work" sheetId="7" r:id="rId7"/>
+    <sheet name="All_contacts_school" sheetId="8" r:id="rId8"/>
+    <sheet name="All_contacts_other" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="16">
   <si>
     <t>[0,5)</t>
   </si>
@@ -433,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A938928-AC38-4BCE-954D-A3A27C30D5E8}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D8D6F-3D64-4D43-A77A-C5358C64EABC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12:H19"/>
     </sheetView>
   </sheetViews>
@@ -1570,4 +1574,1096 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC9941F-5B71-4D8D-B933-B56CE9EB1DA5}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>9.7560975609756101E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.27804878048780501</v>
+      </c>
+      <c r="D4">
+        <v>0.84878048780487803</v>
+      </c>
+      <c r="E4">
+        <v>6.3414634146341506E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.30731707317073198</v>
+      </c>
+      <c r="G4">
+        <v>0.27317073170731698</v>
+      </c>
+      <c r="H4">
+        <v>2.92682926829268E-2</v>
+      </c>
+      <c r="I4">
+        <v>3.4146341463414602E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.178988326848249</v>
+      </c>
+      <c r="C5">
+        <v>0.39688715953307402</v>
+      </c>
+      <c r="D5">
+        <v>0.57976653696498104</v>
+      </c>
+      <c r="E5">
+        <v>0.369649805447471</v>
+      </c>
+      <c r="F5">
+        <v>6.2256809338521402E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.101167315175097</v>
+      </c>
+      <c r="H5">
+        <v>5.0583657587548597E-2</v>
+      </c>
+      <c r="I5">
+        <v>5.4474708171206199E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>7.9295154185022004E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.64317180616740099</v>
+      </c>
+      <c r="D6">
+        <v>0.14977973568281899</v>
+      </c>
+      <c r="E6">
+        <v>0.3215859030837</v>
+      </c>
+      <c r="F6">
+        <v>0.45374449339207001</v>
+      </c>
+      <c r="G6">
+        <v>7.0484581497797405E-2</v>
+      </c>
+      <c r="H6">
+        <v>3.5242290748898703E-2</v>
+      </c>
+      <c r="I6">
+        <v>5.2863436123347998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.3824884792626699E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.29493087557603698</v>
+      </c>
+      <c r="D7">
+        <v>0.26728110599078297</v>
+      </c>
+      <c r="E7">
+        <v>8.2949308755760398E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.43778801843317999</v>
+      </c>
+      <c r="G7">
+        <v>0.33179723502304098</v>
+      </c>
+      <c r="H7">
+        <v>3.2258064516128997E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.101382488479263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3.77358490566038E-3</v>
+      </c>
+      <c r="C8">
+        <v>4.5283018867924497E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.13962264150943399</v>
+      </c>
+      <c r="E8">
+        <v>0.109433962264151</v>
+      </c>
+      <c r="F8">
+        <v>4.5283018867924497E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.43018867924528298</v>
+      </c>
+      <c r="H8">
+        <v>0.354716981132075</v>
+      </c>
+      <c r="I8">
+        <v>0.128301886792453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="E9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F9">
+        <v>7.2916666666666699E-2</v>
+      </c>
+      <c r="G9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.14583333333333301</v>
+      </c>
+      <c r="I9">
+        <v>0.77083333333333304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E5D6EB-31B9-4D60-99DF-C66CAEAF4620}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>9.6618357487922701E-3</v>
+      </c>
+      <c r="C4">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.15942028985507201</v>
+      </c>
+      <c r="E4">
+        <v>0.101449275362319</v>
+      </c>
+      <c r="F4">
+        <v>3.8647342995169101E-2</v>
+      </c>
+      <c r="G4">
+        <v>2.8985507246376802E-2</v>
+      </c>
+      <c r="H4">
+        <v>1.9323671497584499E-2</v>
+      </c>
+      <c r="I4">
+        <v>9.6618357487922701E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3.7037037037036999E-3</v>
+      </c>
+      <c r="C5">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.23703703703703699</v>
+      </c>
+      <c r="E5">
+        <v>0.203703703703704</v>
+      </c>
+      <c r="F5">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="G5">
+        <v>7.7777777777777807E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.48148148148148E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.48148148148148E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>4.1493775933610002E-3</v>
+      </c>
+      <c r="D6">
+        <v>0.128630705394191</v>
+      </c>
+      <c r="E6">
+        <v>0.14937759336099601</v>
+      </c>
+      <c r="F6">
+        <v>0.182572614107884</v>
+      </c>
+      <c r="G6">
+        <v>0.141078838174274</v>
+      </c>
+      <c r="H6">
+        <v>8.29875518672199E-3</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>4.3859649122806998E-3</v>
+      </c>
+      <c r="D7">
+        <v>0.118421052631579</v>
+      </c>
+      <c r="E7">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F7">
+        <v>0.162280701754386</v>
+      </c>
+      <c r="G7">
+        <v>0.157894736842105</v>
+      </c>
+      <c r="H7">
+        <v>8.7719298245613996E-3</v>
+      </c>
+      <c r="I7">
+        <v>2.1929824561403501E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5.4151624548736503E-2</v>
+      </c>
+      <c r="E8">
+        <v>8.6642599277978294E-2</v>
+      </c>
+      <c r="F8">
+        <v>6.4981949458483707E-2</v>
+      </c>
+      <c r="G8">
+        <v>4.6931407942238303E-2</v>
+      </c>
+      <c r="H8">
+        <v>7.2202166064982004E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.4440433212996401E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861D32BE-A58D-4834-ABAC-88187F024C5A}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.6948356807511703E-3</v>
+      </c>
+      <c r="C4">
+        <v>9.3896713615023494E-3</v>
+      </c>
+      <c r="D4">
+        <v>9.3896713615023494E-3</v>
+      </c>
+      <c r="E4">
+        <v>9.3896713615023494E-3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4.6948356807511703E-3</v>
+      </c>
+      <c r="H4">
+        <v>4.6948356807511703E-3</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3.6363636363636398E-3</v>
+      </c>
+      <c r="C5">
+        <v>3.6363636363636398E-3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>3.6363636363636398E-3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>7.2727272727272701E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2D4A9A-FD17-41BB-B5AF-89FACC9EF3FF}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.53061224489796E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.5510204081632699E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.17857142857142899</v>
+      </c>
+      <c r="E4">
+        <v>3.5714285714285698E-2</v>
+      </c>
+      <c r="F4">
+        <v>7.6530612244898003E-2</v>
+      </c>
+      <c r="G4">
+        <v>2.5510204081632699E-2</v>
+      </c>
+      <c r="H4">
+        <v>1.02040816326531E-2</v>
+      </c>
+      <c r="I4">
+        <v>2.04081632653061E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2.0746887966804999E-2</v>
+      </c>
+      <c r="C5">
+        <v>2.4896265560166001E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.10788381742738599</v>
+      </c>
+      <c r="E5">
+        <v>5.8091286307053902E-2</v>
+      </c>
+      <c r="F5">
+        <v>5.39419087136929E-2</v>
+      </c>
+      <c r="G5">
+        <v>4.5643153526971E-2</v>
+      </c>
+      <c r="H5">
+        <v>8.29875518672199E-3</v>
+      </c>
+      <c r="I5">
+        <v>2.9045643153527E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.3698630136986301E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.2831050228310501E-2</v>
+      </c>
+      <c r="D6">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="E6">
+        <v>7.7625570776255703E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.11872146118721499</v>
+      </c>
+      <c r="G6">
+        <v>5.4794520547945202E-2</v>
+      </c>
+      <c r="H6">
+        <v>2.7397260273972601E-2</v>
+      </c>
+      <c r="I6">
+        <v>4.1095890410958902E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.04712041884817E-2</v>
+      </c>
+      <c r="C7">
+        <v>2.6178010471204199E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.104712041884817</v>
+      </c>
+      <c r="E7">
+        <v>8.3769633507853394E-2</v>
+      </c>
+      <c r="F7">
+        <v>8.9005235602094196E-2</v>
+      </c>
+      <c r="G7">
+        <v>9.4240837696335095E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.04712041884817E-2</v>
+      </c>
+      <c r="I7">
+        <v>8.3769633507853394E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.3333333333333299E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.124444444444444</v>
+      </c>
+      <c r="E8">
+        <v>8.4444444444444405E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.10222222222222201</v>
+      </c>
+      <c r="G8">
+        <v>0.11555555555555599</v>
+      </c>
+      <c r="H8">
+        <v>9.3333333333333296E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.3333333333333302E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4.7619047619047603E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="E9">
+        <v>9.5238095238095205E-2</v>
+      </c>
+      <c r="F9">
+        <v>5.95238095238095E-2</v>
+      </c>
+      <c r="G9">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="H9">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>